<commit_message>
Change for Multiple Browser Testing
</commit_message>
<xml_diff>
--- a/cucumber_datadrivenframework_Excel/src/test/resources/testData/default.xlsx
+++ b/cucumber_datadrivenframework_Excel/src/test/resources/testData/default.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5637D6-D314-46AF-A35F-890FF0AEFE6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C602A-7388-46C3-AC19-FC503A08BA10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>abc123</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>Customer service Validation</t>
+  </si>
+  <si>
+    <t>Browsername</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>mozilla</t>
   </si>
 </sst>
 </file>
@@ -450,49 +459,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>